<commit_message>
wczytanie i wizualizacja zeszytu 2
</commit_message>
<xml_diff>
--- a/Wizualizacja i Raportowanie Danych/2016-2017/datasets/Zeszyt2.xlsx
+++ b/Wizualizacja i Raportowanie Danych/2016-2017/datasets/Zeszyt2.xlsx
@@ -1,21 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\vdi-fs01.ue.poznan\Profiles$\36419\Downloads\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="25203"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12440"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
@@ -196,7 +194,7 @@
     <numFmt numFmtId="164" formatCode="@*."/>
     <numFmt numFmtId="165" formatCode="###,###,###.0"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -288,23 +286,23 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom/>
@@ -312,18 +310,18 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top/>
@@ -367,7 +365,7 @@
     <xf numFmtId="4" fontId="2" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Normalny" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normalny_PUBLIK_08_NAKL_" xfId="2"/>
     <cellStyle name="Normalny_PUBLIK_08_Sr_Trw_" xfId="1"/>
   </cellStyles>
@@ -427,7 +425,7 @@
     </a:clrScheme>
     <a:fontScheme name="Pakiet Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -479,7 +477,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -673,7 +671,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -684,24 +682,24 @@
   <dimension ref="A1:P353"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="26.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.85546875" style="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.85546875" style="10" customWidth="1"/>
-    <col min="4" max="4" width="51.7109375" style="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.85546875" style="10" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="41.85546875" style="10" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.28515625" style="10" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="29.85546875" style="10" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.85546875" style="10" customWidth="1"/>
-    <col min="10" max="10" width="10.7109375" style="10" customWidth="1"/>
-    <col min="11" max="11" width="11.5703125" style="10" customWidth="1"/>
-    <col min="12" max="12" width="10.5703125" style="10" customWidth="1"/>
-    <col min="13" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="1" width="26.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.83203125" style="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.83203125" style="10" customWidth="1"/>
+    <col min="4" max="4" width="51.6640625" style="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.83203125" style="10" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="41.83203125" style="10" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.33203125" style="10" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="29.83203125" style="10" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.83203125" style="10" customWidth="1"/>
+    <col min="10" max="10" width="10.6640625" style="10" customWidth="1"/>
+    <col min="11" max="11" width="11.5" style="10" customWidth="1"/>
+    <col min="12" max="12" width="10.5" style="10" customWidth="1"/>
+    <col min="13" max="16384" width="9.1640625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="16.5" customHeight="1">
@@ -856,7 +854,7 @@
       <c r="K5" s="2"/>
       <c r="L5" s="2"/>
     </row>
-    <row r="6" spans="1:16" ht="15.6" customHeight="1">
+    <row r="6" spans="1:16" ht="15.5" customHeight="1">
       <c r="A6" s="17" t="s">
         <v>27</v>
       </c>
@@ -957,7 +955,7 @@
       <c r="O8" s="2"/>
       <c r="P8" s="2"/>
     </row>
-    <row r="9" spans="1:16" s="3" customFormat="1" ht="15.6" customHeight="1">
+    <row r="9" spans="1:16" s="3" customFormat="1" ht="15.5" customHeight="1">
       <c r="A9" s="17" t="s">
         <v>9</v>
       </c>
@@ -1132,7 +1130,7 @@
       <c r="O13" s="2"/>
       <c r="P13" s="2"/>
     </row>
-    <row r="14" spans="1:16" s="3" customFormat="1" ht="15.6" customHeight="1">
+    <row r="14" spans="1:16" s="3" customFormat="1" ht="15.5" customHeight="1">
       <c r="A14" s="17" t="s">
         <v>6</v>
       </c>
@@ -1260,7 +1258,7 @@
       <c r="K17" s="2"/>
       <c r="L17" s="2"/>
     </row>
-    <row r="18" spans="1:12" ht="15.6" customHeight="1">
+    <row r="18" spans="1:12" ht="15.5" customHeight="1">
       <c r="A18" s="17" t="s">
         <v>10</v>
       </c>
@@ -1353,7 +1351,7 @@
       <c r="K20" s="2"/>
       <c r="L20" s="2"/>
     </row>
-    <row r="21" spans="1:12" ht="15.6" customHeight="1">
+    <row r="21" spans="1:12" ht="15.5" customHeight="1">
       <c r="A21" s="17" t="s">
         <v>14</v>
       </c>
@@ -4615,5 +4613,10 @@
     <sortCondition descending="1" ref="B1:B24"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>